<commit_message>
(travail de groupe) finition de la planification
</commit_message>
<xml_diff>
--- a/Documentation/planification.xlsx
+++ b/Documentation/planification.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Joel_Vaucher\INF3-b\Application MVC\Majority\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$O$24</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Cahier des charges</t>
   </si>
@@ -35,9 +38,6 @@
     <t>Documentation</t>
   </si>
   <si>
-    <t>Conception</t>
-  </si>
-  <si>
     <t>Tuto Laravel</t>
   </si>
   <si>
@@ -65,13 +65,43 @@
     <t>Présentation</t>
   </si>
   <si>
-    <t>temps</t>
-  </si>
-  <si>
     <t>Créer/Rejoindre une salle</t>
   </si>
   <si>
-    <t>Push</t>
+    <t>Websocket</t>
+  </si>
+  <si>
+    <t>temps (sem/per)</t>
+  </si>
+  <si>
+    <t>Analyse</t>
+  </si>
+  <si>
+    <t>Conception/réalisation</t>
+  </si>
+  <si>
+    <t>3 pour tous</t>
+  </si>
+  <si>
+    <t>1 pour tous</t>
+  </si>
+  <si>
+    <t>2 pour tous</t>
+  </si>
+  <si>
+    <t>Tous (3x)</t>
+  </si>
+  <si>
+    <t>Joel</t>
+  </si>
+  <si>
+    <t>Julien</t>
+  </si>
+  <si>
+    <t>Vincent</t>
+  </si>
+  <si>
+    <t>responsable</t>
   </si>
 </sst>
 </file>
@@ -95,15 +125,57 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -170,32 +242,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -220,18 +266,42 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -244,9 +314,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -259,7 +327,126 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -268,20 +455,49 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,104 +778,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N26"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.85546875" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" customWidth="1"/>
+    <col min="1" max="1" width="42.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="14" width="7.28515625" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:14" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="10">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="9">
         <v>39</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="10">
         <v>40</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="10">
         <v>42</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="10">
         <v>43</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="10">
         <v>44</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="10">
         <v>45</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="10">
         <v>46</v>
       </c>
-      <c r="J2" s="11">
+      <c r="J2" s="10">
         <v>47</v>
       </c>
-      <c r="K2" s="11">
+      <c r="K2" s="10">
         <v>48</v>
       </c>
-      <c r="L2" s="11">
+      <c r="L2" s="10">
         <v>49</v>
       </c>
-      <c r="M2" s="11">
+      <c r="M2" s="10">
         <v>50</v>
       </c>
-      <c r="N2" s="12">
+      <c r="N2" s="11">
         <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="20"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="B4" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="26"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="15"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="1"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -669,13 +894,15 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
+      <c r="N5" s="12"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="5"/>
+      <c r="A6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="C6" s="3"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -684,185 +911,216 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
+      <c r="N6" s="12"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
+      <c r="A7" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="22"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="25"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="5"/>
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="C8" s="3"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
+      <c r="N8" s="12"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="5"/>
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0.33</v>
+      </c>
       <c r="C9" s="3"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="H9" s="33"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
+      <c r="N9" s="12"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="5"/>
+      <c r="A10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0.33</v>
+      </c>
       <c r="C10" s="3"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="H10" s="33"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
+      <c r="N10" s="12"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="5"/>
+      <c r="A11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0.33</v>
+      </c>
       <c r="C11" s="3"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="H11" s="33"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
+      <c r="N11" s="12"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="5"/>
+      <c r="A12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="6">
+        <v>2</v>
+      </c>
       <c r="C12" s="3"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
+      <c r="N12" s="12"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="5"/>
+      <c r="A13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1</v>
+      </c>
       <c r="C13" s="3"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="H13" s="32"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
+      <c r="N13" s="12"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
+      <c r="A14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6">
+        <v>2</v>
+      </c>
       <c r="C14" s="3"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
+      <c r="N14" s="12"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
+      <c r="A15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="6">
+        <v>1</v>
+      </c>
       <c r="C15" s="3"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="H15" s="30"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
+      <c r="N15" s="12"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
+      <c r="A16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="6">
+        <v>1</v>
+      </c>
       <c r="C16" s="3"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="I16" s="30"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
+      <c r="N16" s="12"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
+      <c r="A17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="6">
+        <v>1</v>
+      </c>
       <c r="C17" s="3"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -870,17 +1128,19 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="J17" s="30"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
+      <c r="N17" s="12"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="5"/>
+      <c r="A18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="6">
+        <v>2</v>
+      </c>
       <c r="C18" s="3"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -889,147 +1149,46 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="N18" s="37"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
+      <c r="A21" s="28" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
+      <c r="A22" s="29" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
+      <c r="A23" s="34" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-    </row>
-    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
+      <c r="A24" s="35" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="M18:N18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="84" orientation="landscape" r:id="rId1"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="33" max="16383" man="1"/>
+  </rowBreaks>
 </worksheet>
 </file>
</xml_diff>